<commit_message>
refine graphics and add 3-agent-model
</commit_message>
<xml_diff>
--- a/simulations/CitizenScience_Calculations_Step1.xlsx
+++ b/simulations/CitizenScience_Calculations_Step1.xlsx
@@ -7,11 +7,12 @@
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Initial Beliefs" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Expected Impacts" sheetId="2" state="visible" r:id="rId2"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Expected Utilities" sheetId="3" state="visible" r:id="rId3"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Belief Update" sheetId="4" state="visible" r:id="rId4"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Exigence Update" sheetId="5" state="visible" r:id="rId5"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Model Parameters" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Initial Beliefs" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Expected Impacts" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Expected Utilities" sheetId="4" state="visible" r:id="rId4"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Belief Update" sheetId="5" state="visible" r:id="rId5"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Exigence Update" sheetId="6" state="visible" r:id="rId6"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -21,7 +22,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="0"/>
-  <fonts count="3">
+  <fonts count="4">
     <font>
       <name val="Calibri"/>
       <family val="2"/>
@@ -35,6 +36,10 @@
     </font>
     <font>
       <b val="1"/>
+    </font>
+    <font>
+      <b val="1"/>
+      <sz val="12"/>
     </font>
   </fonts>
   <fills count="6">
@@ -69,7 +74,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -77,13 +82,22 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
@@ -454,7 +468,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G9"/>
+  <dimension ref="A1:G45"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -465,135 +479,529 @@
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>Initial Beliefs</t>
+          <t>Model Parameters and Assumptions</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="2" t="inlineStr">
         <is>
+          <t>Parameter</t>
+        </is>
+      </c>
+      <c r="B3" s="2" t="inlineStr">
+        <is>
+          <t>Value</t>
+        </is>
+      </c>
+      <c r="C3" s="2" t="inlineStr">
+        <is>
+          <t>Description</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="3" t="inlineStr">
+        <is>
+          <t>Scenario</t>
+        </is>
+      </c>
+      <c r="B4" s="3" t="inlineStr">
+        <is>
+          <t>citizen_science</t>
+        </is>
+      </c>
+      <c r="C4" s="3" t="inlineStr">
+        <is>
+          <t>Generative AI or Citizen Science scenario</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="3" t="inlineStr">
+        <is>
+          <t>M_O</t>
+        </is>
+      </c>
+      <c r="B5" s="3" t="n">
+        <v>0.4</v>
+      </c>
+      <c r="C5" s="3" t="inlineStr">
+        <is>
+          <t>Maximum impact for organization</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="3" t="inlineStr">
+        <is>
+          <t>M_R</t>
+        </is>
+      </c>
+      <c r="B6" s="3" t="n">
+        <v>0.6</v>
+      </c>
+      <c r="C6" s="3" t="inlineStr">
+        <is>
+          <t>Maximum impact for researcher</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="3" t="inlineStr">
+        <is>
+          <t>alpha_O</t>
+        </is>
+      </c>
+      <c r="B7" s="3" t="n">
+        <v>0.6</v>
+      </c>
+      <c r="C7" s="3" t="inlineStr">
+        <is>
+          <t>Weight between impact and private benefit for organization</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="3" t="inlineStr">
+        <is>
+          <t>alpha_R</t>
+        </is>
+      </c>
+      <c r="B8" s="3" t="n">
+        <v>0.7</v>
+      </c>
+      <c r="C8" s="3" t="inlineStr">
+        <is>
+          <t>Weight between impact and private benefit for researcher</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="3" t="inlineStr">
+        <is>
+          <t>P_altruistic</t>
+        </is>
+      </c>
+      <c r="B9" s="3" t="n">
+        <v>0.3</v>
+      </c>
+      <c r="C9" s="3" t="inlineStr">
+        <is>
+          <t>Private benefit for altruistic strategies</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="3" t="inlineStr">
+        <is>
+          <t>P_egoistic</t>
+        </is>
+      </c>
+      <c r="B10" s="3" t="n">
+        <v>0.7</v>
+      </c>
+      <c r="C10" s="3" t="inlineStr">
+        <is>
+          <t>Private benefit for egoistic strategies</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="3" t="inlineStr">
+        <is>
+          <t>X_init</t>
+        </is>
+      </c>
+      <c r="B11" s="3" t="n">
+        <v>0.1845059398261849</v>
+      </c>
+      <c r="C11" s="3" t="inlineStr">
+        <is>
+          <t>Initial exigence value</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="3" t="inlineStr">
+        <is>
+          <t>beta</t>
+        </is>
+      </c>
+      <c r="B12" s="3" t="n">
+        <v>0.3</v>
+      </c>
+      <c r="C12" s="3" t="inlineStr">
+        <is>
+          <t>Learning rate for exigence updates</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="3" t="inlineStr">
+        <is>
+          <t>theta</t>
+        </is>
+      </c>
+      <c r="B13" s="3" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="C13" s="3" t="inlineStr">
+        <is>
+          <t>Threshold impact value</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" s="4" t="inlineStr">
+        <is>
+          <t>Impact Values</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" s="5" t="inlineStr">
+        <is>
+          <t>Organization Impact Values</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" s="5" t="inlineStr">
+        <is>
+          <t>Strategy</t>
+        </is>
+      </c>
+      <c r="B18" s="5" t="inlineStr">
+        <is>
+          <t>Impact</t>
+        </is>
+      </c>
+      <c r="C18" s="5" t="inlineStr">
+        <is>
+          <t>Normalized</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>a,k</t>
+        </is>
+      </c>
+      <c r="B19" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="C19" t="n">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>a,d</t>
+        </is>
+      </c>
+      <c r="B20" t="n">
+        <v>0.7</v>
+      </c>
+      <c r="C20" t="n">
+        <v>0.28</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>a,p</t>
+        </is>
+      </c>
+      <c r="B21" t="n">
+        <v>0.9</v>
+      </c>
+      <c r="C21" t="n">
+        <v>0.36</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>e,k</t>
+        </is>
+      </c>
+      <c r="B22" t="n">
+        <v>0.3</v>
+      </c>
+      <c r="C22" t="n">
+        <v>0.12</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>e,d</t>
+        </is>
+      </c>
+      <c r="B23" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="C23" t="n">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>e,p</t>
+        </is>
+      </c>
+      <c r="B24" t="n">
+        <v>0.6</v>
+      </c>
+      <c r="C24" t="n">
+        <v>0.24</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" s="5" t="inlineStr">
+        <is>
+          <t>Researcher Impact Values</t>
+        </is>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" s="5" t="inlineStr">
+        <is>
+          <t>Strategy</t>
+        </is>
+      </c>
+      <c r="B27" s="5" t="inlineStr">
+        <is>
+          <t>Impact</t>
+        </is>
+      </c>
+      <c r="C27" s="5" t="inlineStr">
+        <is>
+          <t>Normalized</t>
+        </is>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="inlineStr">
+        <is>
+          <t>a,k</t>
+        </is>
+      </c>
+      <c r="B28" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="C28" t="n">
+        <v>0.3</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="inlineStr">
+        <is>
+          <t>a,d</t>
+        </is>
+      </c>
+      <c r="B29" t="n">
+        <v>0.7</v>
+      </c>
+      <c r="C29" t="n">
+        <v>0.42</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="inlineStr">
+        <is>
+          <t>a,p</t>
+        </is>
+      </c>
+      <c r="B30" t="n">
+        <v>0.9</v>
+      </c>
+      <c r="C30" t="n">
+        <v>0.54</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="inlineStr">
+        <is>
+          <t>e,k</t>
+        </is>
+      </c>
+      <c r="B31" t="n">
+        <v>0.3</v>
+      </c>
+      <c r="C31" t="n">
+        <v>0.18</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="inlineStr">
+        <is>
+          <t>e,d</t>
+        </is>
+      </c>
+      <c r="B32" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="C32" t="n">
+        <v>0.3</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="inlineStr">
+        <is>
+          <t>e,p</t>
+        </is>
+      </c>
+      <c r="B33" t="n">
+        <v>0.6</v>
+      </c>
+      <c r="C33" t="n">
+        <v>0.36</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" s="4" t="inlineStr">
+        <is>
+          <t>Current Beliefs</t>
+        </is>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" s="5" t="inlineStr">
+        <is>
+          <t>Updated Beliefs from Previous Step</t>
+        </is>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" s="5" t="inlineStr">
+        <is>
           <t>Organization's beliefs about Researcher strategies</t>
         </is>
       </c>
     </row>
-    <row r="4">
-      <c r="A4" t="inlineStr">
+    <row r="40">
+      <c r="A40" t="inlineStr">
         <is>
           <t>Strategy</t>
         </is>
       </c>
-      <c r="B4" t="inlineStr">
+      <c r="B40" t="inlineStr">
         <is>
           <t>a,k</t>
         </is>
       </c>
-      <c r="C4" t="inlineStr">
+      <c r="C40" t="inlineStr">
         <is>
           <t>a,d</t>
         </is>
       </c>
-      <c r="D4" t="inlineStr">
+      <c r="D40" t="inlineStr">
         <is>
           <t>a,p</t>
         </is>
       </c>
-      <c r="E4" t="inlineStr">
+      <c r="E40" t="inlineStr">
         <is>
           <t>e,k</t>
         </is>
       </c>
-      <c r="F4" t="inlineStr">
+      <c r="F40" t="inlineStr">
         <is>
           <t>e,d</t>
         </is>
       </c>
-      <c r="G4" t="inlineStr">
+      <c r="G40" t="inlineStr">
         <is>
           <t>e,p</t>
         </is>
       </c>
     </row>
-    <row r="5">
-      <c r="B5" t="n">
+    <row r="41">
+      <c r="B41" t="n">
         <v>0.1111111111111111</v>
       </c>
-      <c r="C5" t="n">
+      <c r="C41" t="n">
         <v>0.2177777777777778</v>
       </c>
-      <c r="D5" t="n">
+      <c r="D41" t="n">
         <v>0.3600000000000002</v>
       </c>
-      <c r="E5" t="n">
-        <v>0.04</v>
-      </c>
-      <c r="F5" t="n">
+      <c r="E41" t="n">
+        <v>0.03999999999999999</v>
+      </c>
+      <c r="F41" t="n">
         <v>0.1111111111111111</v>
       </c>
-      <c r="G5" t="n">
+      <c r="G41" t="n">
         <v>0.16</v>
       </c>
     </row>
-    <row r="7">
-      <c r="A7" s="2" t="inlineStr">
+    <row r="43">
+      <c r="A43" s="5" t="inlineStr">
         <is>
           <t>Researcher's beliefs about Organization strategies</t>
         </is>
       </c>
     </row>
-    <row r="8">
-      <c r="A8" t="inlineStr">
+    <row r="44">
+      <c r="A44" t="inlineStr">
         <is>
           <t>Strategy</t>
         </is>
       </c>
-      <c r="B8" t="inlineStr">
+      <c r="B44" t="inlineStr">
         <is>
           <t>a,k</t>
         </is>
       </c>
-      <c r="C8" t="inlineStr">
+      <c r="C44" t="inlineStr">
         <is>
           <t>a,d</t>
         </is>
       </c>
-      <c r="D8" t="inlineStr">
+      <c r="D44" t="inlineStr">
         <is>
           <t>a,p</t>
         </is>
       </c>
-      <c r="E8" t="inlineStr">
+      <c r="E44" t="inlineStr">
         <is>
           <t>e,k</t>
         </is>
       </c>
-      <c r="F8" t="inlineStr">
+      <c r="F44" t="inlineStr">
         <is>
           <t>e,d</t>
         </is>
       </c>
-      <c r="G8" t="inlineStr">
+      <c r="G44" t="inlineStr">
         <is>
           <t>e,p</t>
         </is>
       </c>
     </row>
-    <row r="9">
-      <c r="B9" t="n">
+    <row r="45">
+      <c r="B45" t="n">
         <v>0.1111111111111111</v>
       </c>
-      <c r="C9" t="n">
-        <v>0.2177777777777778</v>
-      </c>
-      <c r="D9" t="n">
+      <c r="C45" t="n">
+        <v>0.2177777777777777</v>
+      </c>
+      <c r="D45" t="n">
         <v>0.3600000000000002</v>
       </c>
-      <c r="E9" t="n">
-        <v>0.04</v>
-      </c>
-      <c r="F9" t="n">
+      <c r="E45" t="n">
+        <v>0.03999999999999999</v>
+      </c>
+      <c r="F45" t="n">
         <v>0.1111111111111111</v>
       </c>
-      <c r="G9" t="n">
+      <c r="G45" t="n">
         <v>0.16</v>
       </c>
     </row>
@@ -619,14 +1027,14 @@
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>Expected Impacts</t>
+          <t>Initial Beliefs</t>
         </is>
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="2" t="inlineStr">
-        <is>
-          <t>Organization's expected impacts</t>
+      <c r="A3" s="5" t="inlineStr">
+        <is>
+          <t>Organization's beliefs about Researcher strategies</t>
         </is>
       </c>
     </row>
@@ -669,28 +1077,28 @@
     </row>
     <row r="5">
       <c r="B5" t="n">
-        <v>0.5977777777777779</v>
+        <v>0.1111111111111111</v>
       </c>
       <c r="C5" t="n">
-        <v>0.6977777777777778</v>
+        <v>0.2177777777777778</v>
       </c>
       <c r="D5" t="n">
-        <v>0.7977777777777779</v>
+        <v>0.3600000000000002</v>
       </c>
       <c r="E5" t="n">
-        <v>0.4977777777777779</v>
+        <v>0.03999999999999999</v>
       </c>
       <c r="F5" t="n">
-        <v>0.5977777777777779</v>
+        <v>0.1111111111111111</v>
       </c>
       <c r="G5" t="n">
-        <v>0.6477777777777778</v>
+        <v>0.16</v>
       </c>
     </row>
     <row r="7">
-      <c r="A7" s="2" t="inlineStr">
-        <is>
-          <t>Researcher's expected impacts</t>
+      <c r="A7" s="5" t="inlineStr">
+        <is>
+          <t>Researcher's beliefs about Organization strategies</t>
         </is>
       </c>
     </row>
@@ -733,22 +1141,22 @@
     </row>
     <row r="9">
       <c r="B9" t="n">
-        <v>0.5977777777777779</v>
+        <v>0.1111111111111111</v>
       </c>
       <c r="C9" t="n">
-        <v>0.6977777777777778</v>
+        <v>0.2177777777777777</v>
       </c>
       <c r="D9" t="n">
-        <v>0.7977777777777779</v>
+        <v>0.3600000000000002</v>
       </c>
       <c r="E9" t="n">
-        <v>0.4977777777777779</v>
+        <v>0.03999999999999999</v>
       </c>
       <c r="F9" t="n">
-        <v>0.5977777777777779</v>
+        <v>0.1111111111111111</v>
       </c>
       <c r="G9" t="n">
-        <v>0.6477777777777778</v>
+        <v>0.16</v>
       </c>
     </row>
   </sheetData>
@@ -773,14 +1181,14 @@
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>Expected Utilities</t>
+          <t>Expected Impacts</t>
         </is>
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="2" t="inlineStr">
-        <is>
-          <t>Organization's expected utilities</t>
+      <c r="A3" s="5" t="inlineStr">
+        <is>
+          <t>Organization's expected impacts</t>
         </is>
       </c>
     </row>
@@ -823,28 +1231,28 @@
     </row>
     <row r="5">
       <c r="B5" t="n">
-        <v>0.4786666666666667</v>
+        <v>0.6173333333333334</v>
       </c>
       <c r="C5" t="n">
-        <v>0.5386666666666666</v>
+        <v>0.6973333333333334</v>
       </c>
       <c r="D5" t="n">
-        <v>0.5986666666666667</v>
+        <v>0.7773333333333334</v>
       </c>
       <c r="E5" t="n">
-        <v>0.5786666666666667</v>
+        <v>0.5373333333333334</v>
       </c>
       <c r="F5" t="n">
-        <v>0.6386666666666667</v>
-      </c>
-      <c r="G5" s="3" t="n">
-        <v>0.6686666666666666</v>
+        <v>0.6173333333333334</v>
+      </c>
+      <c r="G5" t="n">
+        <v>0.6573333333333333</v>
       </c>
     </row>
     <row r="7">
-      <c r="A7" s="2" t="inlineStr">
-        <is>
-          <t>Researcher's expected utilities</t>
+      <c r="A7" s="5" t="inlineStr">
+        <is>
+          <t>Researcher's expected impacts</t>
         </is>
       </c>
     </row>
@@ -887,22 +1295,22 @@
     </row>
     <row r="9">
       <c r="B9" t="n">
-        <v>0.5084444444444445</v>
+        <v>0.5782222222222222</v>
       </c>
       <c r="C9" t="n">
-        <v>0.5784444444444444</v>
+        <v>0.6982222222222223</v>
       </c>
       <c r="D9" t="n">
-        <v>0.6484444444444445</v>
+        <v>0.8182222222222223</v>
       </c>
       <c r="E9" t="n">
-        <v>0.5584444444444445</v>
+        <v>0.4582222222222223</v>
       </c>
       <c r="F9" t="n">
-        <v>0.6284444444444445</v>
-      </c>
-      <c r="G9" s="3" t="n">
-        <v>0.6634444444444445</v>
+        <v>0.5782222222222222</v>
+      </c>
+      <c r="G9" t="n">
+        <v>0.6382222222222222</v>
       </c>
     </row>
   </sheetData>
@@ -911,6 +1319,160 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:G9"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>Expected Utilities</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="5" t="inlineStr">
+        <is>
+          <t>Organization's expected utilities</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>Strategy</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>a,k</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>a,d</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>a,p</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>e,k</t>
+        </is>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>e,d</t>
+        </is>
+      </c>
+      <c r="G4" t="inlineStr">
+        <is>
+          <t>e,p</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="B5" t="n">
+        <v>0.4904</v>
+      </c>
+      <c r="C5" t="n">
+        <v>0.5384</v>
+      </c>
+      <c r="D5" t="n">
+        <v>0.5864</v>
+      </c>
+      <c r="E5" t="n">
+        <v>0.6024</v>
+      </c>
+      <c r="F5" t="n">
+        <v>0.6504</v>
+      </c>
+      <c r="G5" s="6" t="n">
+        <v>0.6743999999999999</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="5" t="inlineStr">
+        <is>
+          <t>Researcher's expected utilities</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>Strategy</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>a,k</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>a,d</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>a,p</t>
+        </is>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>e,k</t>
+        </is>
+      </c>
+      <c r="F8" t="inlineStr">
+        <is>
+          <t>e,d</t>
+        </is>
+      </c>
+      <c r="G8" t="inlineStr">
+        <is>
+          <t>e,p</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="B9" t="n">
+        <v>0.4947555555555556</v>
+      </c>
+      <c r="C9" t="n">
+        <v>0.5787555555555556</v>
+      </c>
+      <c r="D9" s="6" t="n">
+        <v>0.6627555555555555</v>
+      </c>
+      <c r="E9" t="n">
+        <v>0.5307555555555556</v>
+      </c>
+      <c r="F9" t="n">
+        <v>0.6147555555555555</v>
+      </c>
+      <c r="G9" t="n">
+        <v>0.6567555555555555</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -932,7 +1494,7 @@
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="2" t="inlineStr">
+      <c r="A3" s="5" t="inlineStr">
         <is>
           <t>Organization's belief update</t>
         </is>
@@ -972,15 +1534,15 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>0.08466644360479353</v>
+        <v>0.1108765942804184</v>
       </c>
       <c r="C5" t="n">
-        <v>0.009407382622754838</v>
+        <v>0.01231962158671315</v>
       </c>
       <c r="D5" t="n">
-        <v>0.1177804304368906</v>
-      </c>
-      <c r="E5" s="4" t="n">
+        <v>0.1542416622656487</v>
+      </c>
+      <c r="E5" s="7" t="n">
         <v>0.07987220447284343</v>
       </c>
     </row>
@@ -991,16 +1553,16 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>0.1185330210467109</v>
+        <v>0.1552272319925857</v>
       </c>
       <c r="C6" t="n">
-        <v>0.02581385791683927</v>
+        <v>0.03380504163394089</v>
       </c>
       <c r="D6" t="n">
-        <v>0.1177804304368906</v>
-      </c>
-      <c r="E6" s="5" t="n">
-        <v>0.2191693290734823</v>
+        <v>0.1542416622656487</v>
+      </c>
+      <c r="E6" s="8" t="n">
+        <v>0.2191693290734824</v>
       </c>
     </row>
     <row r="7">
@@ -1010,16 +1572,16 @@
         </is>
       </c>
       <c r="B7" t="n">
-        <v>0.1523995984886284</v>
+        <v>0.1995778697047531</v>
       </c>
       <c r="C7" t="n">
-        <v>0.05486385545590624</v>
+        <v>0.07184803309371116</v>
       </c>
       <c r="D7" t="n">
-        <v>0.1177804304368906</v>
-      </c>
-      <c r="E7" s="5" t="n">
-        <v>0.4658146964856231</v>
+        <v>0.1542416622656487</v>
+      </c>
+      <c r="E7" s="9" t="n">
+        <v>0.4658146964856232</v>
       </c>
     </row>
     <row r="8">
@@ -1029,15 +1591,15 @@
         </is>
       </c>
       <c r="B8" t="n">
-        <v>0.05079986616287612</v>
+        <v>0.06652595656825103</v>
       </c>
       <c r="C8" t="n">
-        <v>0.002031994646515045</v>
+        <v>0.002661038262730041</v>
       </c>
       <c r="D8" t="n">
-        <v>0.1177804304368906</v>
-      </c>
-      <c r="E8" s="4" t="n">
+        <v>0.1542416622656487</v>
+      </c>
+      <c r="E8" s="7" t="n">
         <v>0.01725239616613418</v>
       </c>
     </row>
@@ -1048,15 +1610,15 @@
         </is>
       </c>
       <c r="B9" t="n">
-        <v>0.08466644360479353</v>
+        <v>0.1108765942804184</v>
       </c>
       <c r="C9" t="n">
-        <v>0.009407382622754838</v>
+        <v>0.01231962158671315</v>
       </c>
       <c r="D9" t="n">
-        <v>0.1177804304368906</v>
-      </c>
-      <c r="E9" s="4" t="n">
+        <v>0.1542416622656487</v>
+      </c>
+      <c r="E9" s="7" t="n">
         <v>0.07987220447284343</v>
       </c>
     </row>
@@ -1067,15 +1629,15 @@
         </is>
       </c>
       <c r="B10" t="n">
-        <v>0.1015997323257522</v>
+        <v>0.1330519131365021</v>
       </c>
       <c r="C10" t="n">
-        <v>0.01625595717212036</v>
+        <v>0.02128830610184032</v>
       </c>
       <c r="D10" t="n">
-        <v>0.1177804304368906</v>
-      </c>
-      <c r="E10" s="6" t="n">
+        <v>0.1542416622656487</v>
+      </c>
+      <c r="E10" s="7" t="n">
         <v>0.1380191693290734</v>
       </c>
     </row>
@@ -1086,11 +1648,11 @@
         </is>
       </c>
       <c r="E11" t="n">
-        <v>0.9999999999999999</v>
+        <v>1</v>
       </c>
     </row>
     <row r="13">
-      <c r="A13" s="2" t="inlineStr">
+      <c r="A13" s="5" t="inlineStr">
         <is>
           <t>Researcher's belief update</t>
         </is>
@@ -1130,15 +1692,15 @@
         </is>
       </c>
       <c r="B15" t="n">
-        <v>0.08466644360479353</v>
+        <v>0.1108765942804184</v>
       </c>
       <c r="C15" t="n">
-        <v>0.009407382622754838</v>
+        <v>0.01231962158671315</v>
       </c>
       <c r="D15" t="n">
-        <v>0.1177804304368906</v>
-      </c>
-      <c r="E15" s="4" t="n">
+        <v>0.1542416622656487</v>
+      </c>
+      <c r="E15" s="7" t="n">
         <v>0.07987220447284343</v>
       </c>
     </row>
@@ -1149,15 +1711,15 @@
         </is>
       </c>
       <c r="B16" t="n">
-        <v>0.1185330210467109</v>
+        <v>0.1552272319925857</v>
       </c>
       <c r="C16" t="n">
-        <v>0.02581385791683927</v>
+        <v>0.03380504163394087</v>
       </c>
       <c r="D16" t="n">
-        <v>0.1177804304368906</v>
-      </c>
-      <c r="E16" s="5" t="n">
+        <v>0.1542416622656487</v>
+      </c>
+      <c r="E16" s="8" t="n">
         <v>0.2191693290734823</v>
       </c>
     </row>
@@ -1168,16 +1730,16 @@
         </is>
       </c>
       <c r="B17" t="n">
-        <v>0.1523995984886284</v>
+        <v>0.1995778697047531</v>
       </c>
       <c r="C17" t="n">
-        <v>0.05486385545590624</v>
+        <v>0.07184803309371116</v>
       </c>
       <c r="D17" t="n">
-        <v>0.1177804304368906</v>
-      </c>
-      <c r="E17" s="5" t="n">
-        <v>0.4658146964856231</v>
+        <v>0.1542416622656487</v>
+      </c>
+      <c r="E17" s="8" t="n">
+        <v>0.4658146964856232</v>
       </c>
     </row>
     <row r="18">
@@ -1187,15 +1749,15 @@
         </is>
       </c>
       <c r="B18" t="n">
-        <v>0.05079986616287612</v>
+        <v>0.06652595656825103</v>
       </c>
       <c r="C18" t="n">
-        <v>0.002031994646515045</v>
+        <v>0.002661038262730041</v>
       </c>
       <c r="D18" t="n">
-        <v>0.1177804304368906</v>
-      </c>
-      <c r="E18" s="4" t="n">
+        <v>0.1542416622656487</v>
+      </c>
+      <c r="E18" s="7" t="n">
         <v>0.01725239616613418</v>
       </c>
     </row>
@@ -1206,15 +1768,15 @@
         </is>
       </c>
       <c r="B19" t="n">
-        <v>0.08466644360479353</v>
+        <v>0.1108765942804184</v>
       </c>
       <c r="C19" t="n">
-        <v>0.009407382622754838</v>
+        <v>0.01231962158671315</v>
       </c>
       <c r="D19" t="n">
-        <v>0.1177804304368906</v>
-      </c>
-      <c r="E19" s="4" t="n">
+        <v>0.1542416622656487</v>
+      </c>
+      <c r="E19" s="7" t="n">
         <v>0.07987220447284343</v>
       </c>
     </row>
@@ -1225,15 +1787,15 @@
         </is>
       </c>
       <c r="B20" t="n">
-        <v>0.1015997323257522</v>
+        <v>0.1330519131365021</v>
       </c>
       <c r="C20" t="n">
-        <v>0.01625595717212036</v>
+        <v>0.02128830610184032</v>
       </c>
       <c r="D20" t="n">
-        <v>0.1177804304368906</v>
-      </c>
-      <c r="E20" s="6" t="n">
+        <v>0.1542416622656487</v>
+      </c>
+      <c r="E20" s="9" t="n">
         <v>0.1380191693290734</v>
       </c>
     </row>
@@ -1252,7 +1814,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -1280,7 +1842,7 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>0.2010639132117414</v>
+        <v>0.2507623712352219</v>
       </c>
       <c r="C3" t="inlineStr">
         <is>
@@ -1288,7 +1850,7 @@
         </is>
       </c>
       <c r="D3" t="n">
-        <v>0.6477777777777778</v>
+        <v>0.6573333333333333</v>
       </c>
     </row>
     <row r="4">
@@ -1298,7 +1860,7 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>0.3916011920218134</v>
+        <v>0.5253737887277068</v>
       </c>
       <c r="C4" t="inlineStr">
         <is>
@@ -1306,7 +1868,7 @@
         </is>
       </c>
       <c r="D4" t="n">
-        <v>0.6477777777777778</v>
+        <v>0.8182222222222223</v>
       </c>
     </row>
     <row r="5">
@@ -1316,7 +1878,7 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>0.5926651052335548</v>
+        <v>0.7761361599629287</v>
       </c>
       <c r="C5" t="inlineStr">
         <is>
@@ -1324,7 +1886,7 @@
         </is>
       </c>
       <c r="D5" t="n">
-        <v>1.295555555555556</v>
+        <v>1.475555555555556</v>
       </c>
     </row>
     <row r="7">
@@ -1334,7 +1896,7 @@
         </is>
       </c>
       <c r="B7" t="n">
-        <v>0.4673429539736775</v>
+        <v>0.1845059398261849</v>
       </c>
     </row>
     <row r="8">
@@ -1344,7 +1906,7 @@
         </is>
       </c>
       <c r="B8" t="n">
-        <v>0.4382012923537235</v>
+        <v>0.1720414160609027</v>
       </c>
     </row>
     <row r="9">
@@ -1353,8 +1915,8 @@
           <t>Exigence Change</t>
         </is>
       </c>
-      <c r="B9" s="4" t="n">
-        <v>-0.02914166161995396</v>
+      <c r="B9" s="7" t="n">
+        <v>-0.01246452376528215</v>
       </c>
       <c r="C9" t="inlineStr">
         <is>

</xml_diff>